<commit_message>
create aquaculture category in OSPAR
</commit_message>
<xml_diff>
--- a/data/beach_litter/ospar/OSPAR_meta_litter_categories.xlsx
+++ b/data/beach_litter/ospar/OSPAR_meta_litter_categories.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="176">
   <si>
     <t xml:space="preserve">OSPAR</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">MICRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aquaculture</t>
   </si>
   <si>
     <t xml:space="preserve">Comments</t>
@@ -696,13 +699,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T148"/>
+  <dimension ref="A1:U148"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="S27" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="topRight" activeCell="T38" activeCellId="0" sqref="T38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.63"/>
@@ -723,7 +728,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="63.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="20.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="63.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,13 +793,16 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -857,15 +866,19 @@
       </c>
       <c r="S2" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A2), 1)), $C2=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A2), 1)), $C2=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
@@ -929,15 +942,19 @@
       </c>
       <c r="S3" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A3), 1)), $C3=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A3), 1)), $C3=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -1001,15 +1018,19 @@
       </c>
       <c r="S4" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A4), 1)), $C4=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A4), 1)), $C4=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
@@ -1073,15 +1094,19 @@
       </c>
       <c r="S5" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A5), 1)), $C5=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T5" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A5), 1)), $C5=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -1145,15 +1170,19 @@
       </c>
       <c r="S6" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A6), 1)), $C6=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T6" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A6), 1)), $C6=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -1217,15 +1246,19 @@
       </c>
       <c r="S7" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A7), 1)), $C7=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A7), 1)), $C7=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
@@ -1289,15 +1322,19 @@
       </c>
       <c r="S8" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A8), 1)), $C8=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A8), 1)), $C8=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
@@ -1361,15 +1398,19 @@
       </c>
       <c r="S9" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A9), 1)), $C9=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A9), 1)), $C9=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1</v>
@@ -1433,15 +1474,19 @@
       </c>
       <c r="S10" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A10), 1)), $C10=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A10), 1)), $C10=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
@@ -1505,15 +1550,19 @@
       </c>
       <c r="S11" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A11), 1)), $C11=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A11), 1)), $C11=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -1577,15 +1626,19 @@
       </c>
       <c r="S12" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A12), 1)), $C12=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A12), 1)), $C12=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>1</v>
@@ -1649,15 +1702,19 @@
       </c>
       <c r="S13" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A13), 1)), $C13=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A13), 1)), $C13=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>1</v>
@@ -1721,15 +1778,19 @@
       </c>
       <c r="S14" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A14), 1)), $C14=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A14), 1)), $C14=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1</v>
@@ -1793,15 +1854,19 @@
       </c>
       <c r="S15" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A15), 1)), $C15=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A15), 1)), $C15=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>1</v>
@@ -1865,15 +1930,19 @@
       </c>
       <c r="S16" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A16), 1)), $C16=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T16" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A16), 1)), $C16=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>1</v>
@@ -1937,15 +2006,19 @@
       </c>
       <c r="S17" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A17), 1)), $C17=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A17), 1)), $C17=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>1</v>
@@ -2009,15 +2082,19 @@
       </c>
       <c r="S18" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A18), 1)), $C18=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T18" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A18), 1)), $C18=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1</v>
@@ -2081,15 +2158,19 @@
       </c>
       <c r="S19" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A19), 1)), $C19=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A19), 1)), $C19=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1</v>
@@ -2153,15 +2234,19 @@
       </c>
       <c r="S20" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A20), 1)), $C20=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T20" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A20), 1)), $C20=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>1</v>
@@ -2225,15 +2310,19 @@
       </c>
       <c r="S21" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A21), 1)), $C21=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A21), 1)), $C21=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1</v>
@@ -2297,15 +2386,19 @@
       </c>
       <c r="S22" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A22), 1)), $C22=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A22), 1)), $C22=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>1</v>
@@ -2369,15 +2462,19 @@
       </c>
       <c r="S23" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A23), 1)), $C23=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T23" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A23), 1)), $C23=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>1</v>
@@ -2441,15 +2538,19 @@
       </c>
       <c r="S24" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A24), 1)), $C24=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T24" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A24), 1)), $C24=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>1</v>
@@ -2513,15 +2614,19 @@
       </c>
       <c r="S25" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A25), 1)), $C25=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T25" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A25), 1)), $C25=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>1</v>
@@ -2585,15 +2690,19 @@
       </c>
       <c r="S26" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A26), 1)), $C26=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T26" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A26), 1)), $C26=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>1</v>
@@ -2657,15 +2766,19 @@
       </c>
       <c r="S27" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A27), 1)), $C27=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T27" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A27), 1)), $C27=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>1</v>
@@ -2729,15 +2842,19 @@
       </c>
       <c r="S28" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A28), 1)), $C28=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T28" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A28), 1)), $C28=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>1</v>
@@ -2801,15 +2918,19 @@
       </c>
       <c r="S29" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A29), 1)), $C29=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T29" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A29), 1)), $C29=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>1</v>
@@ -2874,14 +2995,17 @@
       <c r="S30" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A30), 1)), $C30=1), 1, 0)</f>
         <v>0</v>
+      </c>
+      <c r="T30" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>1</v>
@@ -2945,15 +3069,19 @@
       </c>
       <c r="S31" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A31), 1)), $C31=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T31" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A31), 1)), $C31=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>1</v>
@@ -3018,14 +3146,17 @@
       <c r="S32" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A32), 1)), $C32=1), 1, 0)</f>
         <v>0</v>
+      </c>
+      <c r="T32" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>1</v>
@@ -3090,14 +3221,17 @@
       <c r="S33" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A33), 1)), $C33=1), 1, 0)</f>
         <v>0</v>
+      </c>
+      <c r="T33" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>1</v>
@@ -3162,14 +3296,17 @@
       <c r="S34" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A34), 1)), $C34=1), 1, 0)</f>
         <v>0</v>
+      </c>
+      <c r="T34" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>1</v>
@@ -3233,15 +3370,19 @@
       </c>
       <c r="S35" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A35), 1)), $C35=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T35" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A35), 1)), $C35=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>1</v>
@@ -3305,15 +3446,19 @@
       </c>
       <c r="S36" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A36), 1)), $C36=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T36" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A36), 1)), $C36=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>1</v>
@@ -3377,15 +3522,19 @@
       </c>
       <c r="S37" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A37), 1)), $C37=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T37" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A37), 1)), $C37=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>1</v>
@@ -3449,15 +3598,19 @@
       </c>
       <c r="S38" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A38), 1)), $C38=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T38" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A38), 1)), $C38=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>1</v>
@@ -3521,15 +3674,19 @@
       </c>
       <c r="S39" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A39), 1)), $C39=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T39" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A39), 1)), $C39=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>1</v>
@@ -3593,15 +3750,19 @@
       </c>
       <c r="S40" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A40), 1)), $C40=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T40" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A40), 1)), $C40=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>1</v>
@@ -3665,15 +3826,19 @@
       </c>
       <c r="S41" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A41), 1)), $C41=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T41" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A41), 1)), $C41=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>1</v>
@@ -3737,15 +3902,19 @@
       </c>
       <c r="S42" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A42), 1)), $C42=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T42" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A42), 1)), $C42=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>1</v>
@@ -3809,15 +3978,19 @@
       </c>
       <c r="S43" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A43), 1)), $C43=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T43" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A43), 1)), $C43=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>1</v>
@@ -3881,15 +4054,19 @@
       </c>
       <c r="S44" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A44), 1)), $C44=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T44" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A44), 1)), $C44=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>1</v>
@@ -3953,15 +4130,19 @@
       </c>
       <c r="S45" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A45), 1)), $C45=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T45" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A45), 1)), $C45=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>1</v>
@@ -4025,15 +4206,19 @@
       </c>
       <c r="S46" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A46), 1)), $C46=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T46" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A46), 1)), $C46=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>1</v>
@@ -4097,15 +4282,19 @@
       </c>
       <c r="S47" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A47), 1)), $C47=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T47" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A47), 1)), $C47=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>1</v>
@@ -4169,15 +4358,19 @@
       </c>
       <c r="S48" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A48), 1)), $C48=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T48" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A48), 1)), $C48=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>1</v>
@@ -4241,15 +4434,19 @@
       </c>
       <c r="S49" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A49), 1)), $C49=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T49" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A49), 1)), $C49=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>1</v>
@@ -4313,15 +4510,19 @@
       </c>
       <c r="S50" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A50), 1)), $C50=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T50" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A50), 1)), $C50=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>1</v>
@@ -4385,15 +4586,19 @@
       </c>
       <c r="S51" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A51), 1)), $C51=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T51" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A51), 1)), $C51=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C52" s="4" t="n">
         <v>0</v>
@@ -4458,16 +4663,20 @@
       <c r="S52" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="T52" s="4" t="s">
-        <v>74</v>
+      <c r="T52" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A52), 1)), $C52=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U52" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>1</v>
@@ -4531,15 +4740,19 @@
       </c>
       <c r="S53" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A53), 1)), $C53=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T53" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A53), 1)), $C53=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>1</v>
@@ -4603,15 +4816,19 @@
       </c>
       <c r="S54" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A54), 1)), $C54=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T54" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A54), 1)), $C54=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>1</v>
@@ -4675,15 +4892,19 @@
       </c>
       <c r="S55" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A55), 1)), $C55=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T55" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A55), 1)), $C55=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>1</v>
@@ -4747,15 +4968,19 @@
       </c>
       <c r="S56" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A56), 1)), $C56=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T56" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A56), 1)), $C56=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>1</v>
@@ -4819,15 +5044,19 @@
       </c>
       <c r="S57" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A57), 1)), $C57=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T57" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A57), 1)), $C57=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>1</v>
@@ -4891,15 +5120,19 @@
       </c>
       <c r="S58" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A58), 1)), $C58=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T58" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A58), 1)), $C58=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>1</v>
@@ -4963,15 +5196,19 @@
       </c>
       <c r="S59" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A59), 1)), $C59=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T59" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A59), 1)), $C59=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>1</v>
@@ -5035,15 +5272,19 @@
       </c>
       <c r="S60" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A60), 1)), $C60=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T60" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A60), 1)), $C60=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>1</v>
@@ -5107,15 +5348,19 @@
       </c>
       <c r="S61" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A61), 1)), $C61=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T61" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A61), 1)), $C61=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>1</v>
@@ -5179,15 +5424,19 @@
       </c>
       <c r="S62" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A62), 1)), $C62=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T62" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A62), 1)), $C62=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C63" s="0" t="n">
         <v>1</v>
@@ -5251,15 +5500,19 @@
       </c>
       <c r="S63" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A63), 1)), $C63=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T63" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A63), 1)), $C63=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>1</v>
@@ -5323,15 +5576,19 @@
       </c>
       <c r="S64" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A64), 1)), $C64=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T64" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A64), 1)), $C64=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>1</v>
@@ -5395,15 +5652,19 @@
       </c>
       <c r="S65" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A65), 1)), $C65=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T65" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A65), 1)), $C65=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B66" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>88</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>1</v>
@@ -5467,15 +5728,19 @@
       </c>
       <c r="S66" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A66), 1)), $C66=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T66" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A66), 1)), $C66=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C67" s="0" t="n">
         <v>1</v>
@@ -5539,15 +5804,19 @@
       </c>
       <c r="S67" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A67), 1)), $C67=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T67" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A67), 1)), $C67=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>1</v>
@@ -5611,15 +5880,19 @@
       </c>
       <c r="S68" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A68), 1)), $C68=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T68" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A68), 1)), $C68=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>1</v>
@@ -5683,12 +5956,16 @@
       </c>
       <c r="S69" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A69), 1)), $C69=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T69" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A69), 1)), $C69=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>5</v>
@@ -5755,15 +6032,19 @@
       </c>
       <c r="S70" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A70), 1)), $C70=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T70" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A70), 1)), $C70=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C71" s="0" t="n">
         <v>1</v>
@@ -5827,15 +6108,19 @@
       </c>
       <c r="S71" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A71), 1)), $C71=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T71" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A71), 1)), $C71=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C72" s="0" t="n">
         <v>1</v>
@@ -5899,15 +6184,19 @@
       </c>
       <c r="S72" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A72), 1)), $C72=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T72" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A72), 1)), $C72=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C73" s="0" t="n">
         <v>1</v>
@@ -5971,15 +6260,19 @@
       </c>
       <c r="S73" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A73), 1)), $C73=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T73" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A73), 1)), $C73=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C74" s="0" t="n">
         <v>1</v>
@@ -6043,15 +6336,19 @@
       </c>
       <c r="S74" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A74), 1)), $C74=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T74" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A74), 1)), $C74=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>1</v>
@@ -6115,15 +6412,19 @@
       </c>
       <c r="S75" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A75), 1)), $C75=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T75" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A75), 1)), $C75=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C76" s="0" t="n">
         <v>1</v>
@@ -6187,15 +6488,19 @@
       </c>
       <c r="S76" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A76), 1)), $C76=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T76" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A76), 1)), $C76=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C77" s="0" t="n">
         <v>1</v>
@@ -6259,15 +6564,19 @@
       </c>
       <c r="S77" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A77), 1)), $C77=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T77" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A77), 1)), $C77=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C78" s="0" t="n">
         <v>1</v>
@@ -6331,15 +6640,19 @@
       </c>
       <c r="S78" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A78), 1)), $C78=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T78" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A78), 1)), $C78=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C79" s="0" t="n">
         <v>1</v>
@@ -6403,15 +6716,19 @@
       </c>
       <c r="S79" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A79), 1)), $C79=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T79" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A79), 1)), $C79=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C80" s="0" t="n">
         <v>1</v>
@@ -6475,15 +6792,19 @@
       </c>
       <c r="S80" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A80), 1)), $C80=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T80" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A80), 1)), $C80=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C81" s="0" t="n">
         <v>1</v>
@@ -6547,15 +6868,19 @@
       </c>
       <c r="S81" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A81), 1)), $C81=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T81" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A81), 1)), $C81=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C82" s="0" t="n">
         <v>1</v>
@@ -6619,15 +6944,19 @@
       </c>
       <c r="S82" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A82), 1)), $C82=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T82" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A82), 1)), $C82=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C83" s="0" t="n">
         <v>1</v>
@@ -6691,15 +7020,19 @@
       </c>
       <c r="S83" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A83), 1)), $C83=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T83" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A83), 1)), $C83=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B84" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="B84" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="C84" s="0" t="n">
         <v>1</v>
@@ -6763,15 +7096,19 @@
       </c>
       <c r="S84" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A84), 1)), $C84=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T84" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A84), 1)), $C84=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C85" s="0" t="n">
         <v>1</v>
@@ -6835,15 +7172,19 @@
       </c>
       <c r="S85" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A85), 1)), $C85=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T85" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A85), 1)), $C85=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C86" s="0" t="n">
         <v>1</v>
@@ -6907,15 +7248,19 @@
       </c>
       <c r="S86" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A86), 1)), $C86=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T86" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A86), 1)), $C86=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C87" s="0" t="n">
         <v>1</v>
@@ -6979,15 +7324,19 @@
       </c>
       <c r="S87" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A87), 1)), $C87=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T87" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A87), 1)), $C87=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C88" s="0" t="n">
         <v>1</v>
@@ -7051,15 +7400,19 @@
       </c>
       <c r="S88" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A88), 1)), $C88=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T88" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A88), 1)), $C88=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C89" s="0" t="n">
         <v>1</v>
@@ -7123,15 +7476,19 @@
       </c>
       <c r="S89" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A89), 1)), $C89=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T89" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A89), 1)), $C89=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>1</v>
@@ -7195,15 +7552,19 @@
       </c>
       <c r="S90" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A90), 1)), $C90=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T90" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A90), 1)), $C90=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C91" s="0" t="n">
         <v>1</v>
@@ -7267,15 +7628,19 @@
       </c>
       <c r="S91" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A91), 1)), $C91=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T91" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A91), 1)), $C91=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C92" s="0" t="n">
         <v>1</v>
@@ -7339,15 +7704,19 @@
       </c>
       <c r="S92" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A92), 1)), $C92=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T92" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A92), 1)), $C92=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C93" s="0" t="n">
         <v>1</v>
@@ -7411,15 +7780,19 @@
       </c>
       <c r="S93" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A93), 1)), $C93=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T93" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A93), 1)), $C93=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C94" s="0" t="n">
         <v>1</v>
@@ -7483,15 +7856,19 @@
       </c>
       <c r="S94" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A94), 1)), $C94=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T94" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A94), 1)), $C94=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C95" s="0" t="n">
         <v>1</v>
@@ -7555,15 +7932,19 @@
       </c>
       <c r="S95" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A95), 1)), $C95=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T95" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A95), 1)), $C95=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C96" s="0" t="n">
         <v>1</v>
@@ -7627,15 +8008,19 @@
       </c>
       <c r="S96" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A96), 1)), $C96=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T96" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A96), 1)), $C96=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C97" s="0" t="n">
         <v>1</v>
@@ -7699,12 +8084,16 @@
       </c>
       <c r="S97" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A97), 1)), $C97=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T97" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A97), 1)), $C97=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>13</v>
@@ -7771,15 +8160,19 @@
       </c>
       <c r="S98" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A98), 1)), $C98=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T98" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A98), 1)), $C98=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C99" s="0" t="n">
         <v>1</v>
@@ -7843,12 +8236,16 @@
       </c>
       <c r="S99" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A99), 1)), $C99=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T99" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A99), 1)), $C99=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>13</v>
@@ -7915,15 +8312,19 @@
       </c>
       <c r="S100" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A100), 1)), $C100=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T100" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A100), 1)), $C100=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C101" s="0" t="n">
         <v>1</v>
@@ -7987,15 +8388,19 @@
       </c>
       <c r="S101" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A101), 1)), $C101=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T101" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A101), 1)), $C101=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C102" s="0" t="n">
         <v>1</v>
@@ -8059,15 +8464,19 @@
       </c>
       <c r="S102" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A102), 1)), $C102=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T102" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A102), 1)), $C102=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C103" s="0" t="n">
         <v>1</v>
@@ -8131,15 +8540,19 @@
       </c>
       <c r="S103" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A103), 1)), $C103=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T103" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A103), 1)), $C103=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C104" s="0" t="n">
         <v>1</v>
@@ -8203,15 +8616,19 @@
       </c>
       <c r="S104" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A104), 1)), $C104=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T104" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A104), 1)), $C104=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C105" s="5" t="n">
         <v>1</v>
@@ -8275,15 +8692,19 @@
       </c>
       <c r="S105" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A105), 1)), $C105=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T105" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A105), 1)), $C105=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C106" s="0" t="n">
         <v>1</v>
@@ -8347,15 +8768,19 @@
       </c>
       <c r="S106" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A106), 1)), $C106=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T106" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A106), 1)), $C106=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C107" s="0" t="n">
         <v>1</v>
@@ -8419,15 +8844,19 @@
       </c>
       <c r="S107" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A107), 1)), $C107=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T107" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A107), 1)), $C107=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C108" s="0" t="n">
         <v>1</v>
@@ -8491,15 +8920,19 @@
       </c>
       <c r="S108" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A108), 1)), $C108=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T108" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A108), 1)), $C108=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C109" s="0" t="n">
         <v>1</v>
@@ -8563,15 +8996,19 @@
       </c>
       <c r="S109" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A109), 1)), $C109=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T109" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A109), 1)), $C109=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C110" s="0" t="n">
         <v>1</v>
@@ -8635,15 +9072,19 @@
       </c>
       <c r="S110" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A110), 1)), $C110=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T110" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A110), 1)), $C110=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C111" s="0" t="n">
         <v>1</v>
@@ -8707,15 +9148,19 @@
       </c>
       <c r="S111" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A111), 1)), $C111=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T111" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A111), 1)), $C111=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C112" s="0" t="n">
         <v>1</v>
@@ -8779,15 +9224,19 @@
       </c>
       <c r="S112" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A112), 1)), $C112=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T112" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A112), 1)), $C112=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C113" s="0" t="n">
         <v>1</v>
@@ -8851,15 +9300,19 @@
       </c>
       <c r="S113" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A113), 1)), $C113=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T113" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A113), 1)), $C113=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C114" s="4" t="n">
         <v>0</v>
@@ -8925,16 +9378,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A114), 1)), $C114=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T114" s="4" t="s">
-        <v>74</v>
+      <c r="T114" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A114), 1)), $C114=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U114" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C115" s="4" t="n">
         <v>0</v>
@@ -8998,15 +9455,19 @@
       </c>
       <c r="S115" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A115), 1)), $C115=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T115" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A115), 1)), $C115=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C116" s="4" t="n">
         <v>0</v>
@@ -9070,15 +9531,19 @@
       </c>
       <c r="S116" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A116), 1)), $C116=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T116" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A116), 1)), $C116=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C117" s="4" t="n">
         <v>0</v>
@@ -9142,15 +9607,19 @@
       </c>
       <c r="S117" s="2" t="n">
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A117), 1)), $C117=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T117" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A117), 1)), $C117=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C118" s="4" t="n">
         <v>0</v>
@@ -9216,16 +9685,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A118), 1)), $C118=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T118" s="4" t="s">
-        <v>143</v>
+      <c r="T118" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A118), 1)), $C118=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U118" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C119" s="4" t="n">
         <v>0</v>
@@ -9291,16 +9764,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A119), 1)), $C119=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T119" s="4" t="s">
-        <v>143</v>
+      <c r="T119" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A119), 1)), $C119=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U119" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C120" s="4" t="n">
         <v>0</v>
@@ -9366,16 +9843,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A120), 1)), $C120=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T120" s="4" t="s">
-        <v>143</v>
+      <c r="T120" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A120), 1)), $C120=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U120" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C121" s="4" t="n">
         <v>0</v>
@@ -9441,16 +9922,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A121), 1)), $C121=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T121" s="4" t="s">
-        <v>143</v>
+      <c r="T121" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A121), 1)), $C121=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U121" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C122" s="4" t="n">
         <v>0</v>
@@ -9516,16 +10001,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A122), 1)), $C122=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T122" s="4" t="s">
-        <v>143</v>
+      <c r="T122" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A122), 1)), $C122=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U122" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C123" s="4" t="n">
         <v>0</v>
@@ -9591,16 +10080,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A123), 1)), $C123=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T123" s="4" t="s">
-        <v>143</v>
+      <c r="T123" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A123), 1)), $C123=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U123" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C124" s="4" t="n">
         <v>0</v>
@@ -9666,16 +10159,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A124), 1)), $C124=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T124" s="4" t="s">
-        <v>143</v>
+      <c r="T124" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A124), 1)), $C124=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U124" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C125" s="4" t="n">
         <v>0</v>
@@ -9741,16 +10238,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A125), 1)), $C125=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T125" s="4" t="s">
-        <v>143</v>
+      <c r="T125" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A125), 1)), $C125=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U125" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C126" s="4" t="n">
         <v>0</v>
@@ -9816,16 +10317,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A126), 1)), $C126=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T126" s="4" t="s">
-        <v>143</v>
+      <c r="T126" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A126), 1)), $C126=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U126" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C127" s="4" t="n">
         <v>0</v>
@@ -9891,16 +10396,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A127), 1)), $C127=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T127" s="4" t="s">
-        <v>143</v>
+      <c r="T127" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A127), 1)), $C127=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U127" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C128" s="4" t="n">
         <v>0</v>
@@ -9966,16 +10475,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A128), 1)), $C128=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T128" s="4" t="s">
-        <v>143</v>
+      <c r="T128" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A128), 1)), $C128=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U128" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C129" s="4" t="n">
         <v>0</v>
@@ -10041,16 +10554,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A129), 1)), $C129=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T129" s="4" t="s">
-        <v>143</v>
+      <c r="T129" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A129), 1)), $C129=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U129" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C130" s="4" t="n">
         <v>0</v>
@@ -10116,16 +10633,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A130), 1)), $C130=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T130" s="4" t="s">
-        <v>143</v>
+      <c r="T130" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A130), 1)), $C130=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U130" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C131" s="4" t="n">
         <v>0</v>
@@ -10191,16 +10712,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A131), 1)), $C131=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T131" s="4" t="s">
-        <v>143</v>
+      <c r="T131" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A131), 1)), $C131=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U131" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C132" s="4" t="n">
         <v>0</v>
@@ -10266,16 +10791,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A132), 1)), $C132=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T132" s="4" t="s">
-        <v>143</v>
+      <c r="T132" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A132), 1)), $C132=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U132" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C133" s="4" t="n">
         <v>0</v>
@@ -10341,16 +10870,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A133), 1)), $C133=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T133" s="4" t="s">
-        <v>143</v>
+      <c r="T133" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A133), 1)), $C133=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U133" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C134" s="4" t="n">
         <v>0</v>
@@ -10416,16 +10949,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A134), 1)), $C134=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T134" s="4" t="s">
-        <v>143</v>
+      <c r="T134" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A134), 1)), $C134=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U134" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C135" s="4" t="n">
         <v>0</v>
@@ -10491,16 +11028,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A135), 1)), $C135=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T135" s="4" t="s">
-        <v>143</v>
+      <c r="T135" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A135), 1)), $C135=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U135" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C136" s="4" t="n">
         <v>0</v>
@@ -10566,16 +11107,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A136), 1)), $C136=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T136" s="4" t="s">
-        <v>143</v>
+      <c r="T136" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A136), 1)), $C136=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U136" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C137" s="4" t="n">
         <v>0</v>
@@ -10641,16 +11186,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A137), 1)), $C137=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T137" s="4" t="s">
-        <v>143</v>
+      <c r="T137" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A137), 1)), $C137=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U137" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C138" s="4" t="n">
         <v>0</v>
@@ -10716,16 +11265,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A138), 1)), $C138=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T138" s="4" t="s">
-        <v>164</v>
+      <c r="T138" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A138), 1)), $C138=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U138" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C139" s="4" t="n">
         <v>0</v>
@@ -10791,16 +11344,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A139), 1)), $C139=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T139" s="4" t="s">
-        <v>164</v>
+      <c r="T139" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A139), 1)), $C139=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U139" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C140" s="4" t="n">
         <v>0</v>
@@ -10866,16 +11423,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A140), 1)), $C140=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T140" s="4" t="s">
-        <v>164</v>
+      <c r="T140" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A140), 1)), $C140=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U140" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C141" s="4" t="n">
         <v>0</v>
@@ -10941,16 +11502,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A141), 1)), $C141=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T141" s="4" t="s">
-        <v>164</v>
+      <c r="T141" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A141), 1)), $C141=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U141" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C142" s="4" t="n">
         <v>0</v>
@@ -11016,16 +11581,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A142), 1)), $C142=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T142" s="4" t="s">
-        <v>164</v>
+      <c r="T142" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A142), 1)), $C142=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U142" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C143" s="4" t="n">
         <v>0</v>
@@ -11091,16 +11660,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A143), 1)), $C143=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T143" s="4" t="s">
-        <v>164</v>
+      <c r="T143" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A143), 1)), $C143=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U143" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C144" s="4" t="n">
         <v>0</v>
@@ -11166,16 +11739,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A144), 1)), $C144=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T144" s="4" t="s">
-        <v>164</v>
+      <c r="T144" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A144), 1)), $C144=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U144" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C145" s="4" t="n">
         <v>0</v>
@@ -11241,16 +11818,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A145), 1)), $C145=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T145" s="4" t="s">
-        <v>164</v>
+      <c r="T145" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A145), 1)), $C145=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U145" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C146" s="4" t="n">
         <v>0</v>
@@ -11316,16 +11897,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A146), 1)), $C146=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T146" s="4" t="s">
-        <v>164</v>
+      <c r="T146" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A146), 1)), $C146=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U146" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C147" s="4" t="n">
         <v>0</v>
@@ -11391,16 +11976,20 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A147), 1)), $C147=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T147" s="4" t="s">
-        <v>164</v>
+      <c r="T147" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A147), 1)), $C147=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U147" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C148" s="4" t="n">
         <v>0</v>
@@ -11466,8 +12055,12 @@
         <f aca="false">IF(AND(ISNUMBER(FIND(T(S$1), T($A148), 1)), $C148=1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="T148" s="4" t="s">
-        <v>74</v>
+      <c r="T148" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(T$1), T($A148), 1)), $C148=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U148" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -16476,7 +17069,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:S148">
+  <conditionalFormatting sqref="H3:T148 H2:S148 T2">
     <cfRule type="colorScale" priority="772">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
add String as OSPAR meta cateogry
</commit_message>
<xml_diff>
--- a/data/beach_litter/ospar/OSPAR_meta_litter_categories.xlsx
+++ b/data/beach_litter/ospar/OSPAR_meta_litter_categories.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="178">
   <si>
     <t xml:space="preserve">OSPAR</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">Aquaculture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String</t>
   </si>
   <si>
     <t xml:space="preserve">Non-Aqua</t>
@@ -702,15 +705,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V148"/>
+  <dimension ref="A1:W148"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="O2" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="topRight" activeCell="R27" activeCellId="0" sqref="R27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="U15" activeCellId="0" sqref="U15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.63"/>
@@ -732,8 +735,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="20.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="63.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="63.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -803,13 +806,16 @@
       <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -880,15 +886,18 @@
         <v>0</v>
       </c>
       <c r="U2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
@@ -959,15 +968,18 @@
         <v>0</v>
       </c>
       <c r="U3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -1038,15 +1050,18 @@
         <v>0</v>
       </c>
       <c r="U4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
@@ -1117,15 +1132,18 @@
         <v>0</v>
       </c>
       <c r="U5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -1196,15 +1214,18 @@
         <v>0</v>
       </c>
       <c r="U6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -1275,15 +1296,18 @@
         <v>0</v>
       </c>
       <c r="U7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
@@ -1354,15 +1378,18 @@
         <v>0</v>
       </c>
       <c r="U8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
@@ -1433,15 +1460,18 @@
         <v>0</v>
       </c>
       <c r="U9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1</v>
@@ -1512,15 +1542,18 @@
         <v>0</v>
       </c>
       <c r="U10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
@@ -1591,15 +1624,18 @@
         <v>0</v>
       </c>
       <c r="U11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -1670,15 +1706,18 @@
         <v>0</v>
       </c>
       <c r="U12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>1</v>
@@ -1749,15 +1788,18 @@
         <v>0</v>
       </c>
       <c r="U13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>1</v>
@@ -1828,15 +1870,18 @@
         <v>0</v>
       </c>
       <c r="U14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1</v>
@@ -1907,15 +1952,18 @@
         <v>0</v>
       </c>
       <c r="U15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>1</v>
@@ -1986,15 +2034,18 @@
         <v>0</v>
       </c>
       <c r="U16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>1</v>
@@ -2065,15 +2116,18 @@
         <v>0</v>
       </c>
       <c r="U17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>1</v>
@@ -2144,15 +2198,18 @@
         <v>0</v>
       </c>
       <c r="U18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1</v>
@@ -2223,15 +2280,18 @@
         <v>0</v>
       </c>
       <c r="U19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V19" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1</v>
@@ -2302,15 +2362,18 @@
         <v>0</v>
       </c>
       <c r="U20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>1</v>
@@ -2381,15 +2444,18 @@
         <v>0</v>
       </c>
       <c r="U21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1</v>
@@ -2460,15 +2526,18 @@
         <v>0</v>
       </c>
       <c r="U22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>1</v>
@@ -2539,15 +2608,18 @@
         <v>0</v>
       </c>
       <c r="U23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>1</v>
@@ -2618,15 +2690,18 @@
         <v>0</v>
       </c>
       <c r="U24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>1</v>
@@ -2697,15 +2772,18 @@
         <v>0</v>
       </c>
       <c r="U25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>1</v>
@@ -2776,15 +2854,18 @@
         <v>0</v>
       </c>
       <c r="U26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V26" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>1</v>
@@ -2855,15 +2936,18 @@
         <v>0</v>
       </c>
       <c r="U27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>1</v>
@@ -2934,15 +3018,18 @@
         <v>0</v>
       </c>
       <c r="U28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V28" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>1</v>
@@ -3013,15 +3100,18 @@
         <v>0</v>
       </c>
       <c r="U29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V29" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>1</v>
@@ -3091,15 +3181,18 @@
         <v>1</v>
       </c>
       <c r="U30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>1</v>
@@ -3170,15 +3263,18 @@
         <v>0</v>
       </c>
       <c r="U31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>1</v>
@@ -3248,16 +3344,19 @@
         <v>1</v>
       </c>
       <c r="U32" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A32), 1)), $C32=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V32" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A32), 1)), $C32=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>1</v>
@@ -3327,16 +3426,19 @@
         <v>1</v>
       </c>
       <c r="U33" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A33), 1)), $C33=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V33" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A33), 1)), $C33=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>1</v>
@@ -3406,16 +3508,19 @@
         <v>1</v>
       </c>
       <c r="U34" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A34), 1)), $C34=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V34" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A34), 1)), $C34=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>1</v>
@@ -3486,15 +3591,18 @@
         <v>0</v>
       </c>
       <c r="U35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>1</v>
@@ -3565,15 +3673,18 @@
         <v>0</v>
       </c>
       <c r="U36" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V36" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>1</v>
@@ -3644,15 +3755,18 @@
         <v>0</v>
       </c>
       <c r="U37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V37" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>1</v>
@@ -3723,15 +3837,18 @@
         <v>0</v>
       </c>
       <c r="U38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V38" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>1</v>
@@ -3802,15 +3919,18 @@
         <v>0</v>
       </c>
       <c r="U39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V39" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>1</v>
@@ -3881,15 +4001,18 @@
         <v>0</v>
       </c>
       <c r="U40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V40" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>1</v>
@@ -3960,15 +4083,18 @@
         <v>0</v>
       </c>
       <c r="U41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V41" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>1</v>
@@ -4039,15 +4165,18 @@
         <v>0</v>
       </c>
       <c r="U42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V42" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>1</v>
@@ -4118,15 +4247,18 @@
         <v>0</v>
       </c>
       <c r="U43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V43" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>1</v>
@@ -4197,15 +4329,18 @@
         <v>0</v>
       </c>
       <c r="U44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V44" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>1</v>
@@ -4276,15 +4411,18 @@
         <v>0</v>
       </c>
       <c r="U45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V45" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>1</v>
@@ -4355,15 +4493,18 @@
         <v>0</v>
       </c>
       <c r="U46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V46" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>1</v>
@@ -4434,15 +4575,18 @@
         <v>0</v>
       </c>
       <c r="U47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V47" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>1</v>
@@ -4513,15 +4657,18 @@
         <v>0</v>
       </c>
       <c r="U48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V48" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>1</v>
@@ -4592,15 +4739,18 @@
         <v>0</v>
       </c>
       <c r="U49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V49" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>1</v>
@@ -4671,15 +4821,18 @@
         <v>0</v>
       </c>
       <c r="U50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V50" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>1</v>
@@ -4750,15 +4903,18 @@
         <v>0</v>
       </c>
       <c r="U51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V51" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C52" s="4" t="n">
         <v>0</v>
@@ -4830,16 +4986,19 @@
       <c r="U52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="V52" s="4" t="s">
-        <v>76</v>
+      <c r="V52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W52" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>1</v>
@@ -4910,15 +5069,18 @@
         <v>0</v>
       </c>
       <c r="U53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V53" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>1</v>
@@ -4989,15 +5151,18 @@
         <v>0</v>
       </c>
       <c r="U54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V54" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>1</v>
@@ -5068,16 +5233,19 @@
         <v>0</v>
       </c>
       <c r="U55" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A55), 1)), $C55=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V55" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A55), 1)), $C55=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>1</v>
@@ -5148,15 +5316,18 @@
         <v>0</v>
       </c>
       <c r="U56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V56" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>1</v>
@@ -5227,16 +5398,19 @@
         <v>0</v>
       </c>
       <c r="U57" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A57), 1)), $C57=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V57" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A57), 1)), $C57=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>1</v>
@@ -5307,16 +5481,19 @@
         <v>0</v>
       </c>
       <c r="U58" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A58), 1)), $C58=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V58" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A58), 1)), $C58=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>1</v>
@@ -5387,16 +5564,19 @@
         <v>0</v>
       </c>
       <c r="U59" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A59), 1)), $C59=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V59" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A59), 1)), $C59=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>1</v>
@@ -5467,16 +5647,19 @@
         <v>0</v>
       </c>
       <c r="U60" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A60), 1)), $C60=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V60" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A60), 1)), $C60=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>1</v>
@@ -5547,16 +5730,19 @@
         <v>0</v>
       </c>
       <c r="U61" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A61), 1)), $C61=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V61" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A61), 1)), $C61=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>1</v>
@@ -5627,16 +5813,19 @@
         <v>0</v>
       </c>
       <c r="U62" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A62), 1)), $C62=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V62" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A62), 1)), $C62=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C63" s="0" t="n">
         <v>1</v>
@@ -5707,16 +5896,19 @@
         <v>0</v>
       </c>
       <c r="U63" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A63), 1)), $C63=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V63" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A63), 1)), $C63=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>1</v>
@@ -5787,16 +5979,19 @@
         <v>0</v>
       </c>
       <c r="U64" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A64), 1)), $C64=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V64" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A64), 1)), $C64=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>1</v>
@@ -5867,16 +6062,19 @@
         <v>0</v>
       </c>
       <c r="U65" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A65), 1)), $C65=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V65" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A65), 1)), $C65=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B66" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>90</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>1</v>
@@ -5947,16 +6145,19 @@
         <v>0</v>
       </c>
       <c r="U66" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A66), 1)), $C66=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V66" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A66), 1)), $C66=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C67" s="0" t="n">
         <v>1</v>
@@ -6027,16 +6228,19 @@
         <v>0</v>
       </c>
       <c r="U67" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A67), 1)), $C67=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V67" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A67), 1)), $C67=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>1</v>
@@ -6107,16 +6311,19 @@
         <v>0</v>
       </c>
       <c r="U68" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A68), 1)), $C68=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V68" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A68), 1)), $C68=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>1</v>
@@ -6187,13 +6394,16 @@
         <v>0</v>
       </c>
       <c r="U69" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A69), 1)), $C69=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V69" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A69), 1)), $C69=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>5</v>
@@ -6267,16 +6477,19 @@
         <v>0</v>
       </c>
       <c r="U70" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A70), 1)), $C70=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V70" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A70), 1)), $C70=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C71" s="0" t="n">
         <v>1</v>
@@ -6347,16 +6560,19 @@
         <v>0</v>
       </c>
       <c r="U71" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A71), 1)), $C71=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V71" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A71), 1)), $C71=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C72" s="0" t="n">
         <v>1</v>
@@ -6427,16 +6643,19 @@
         <v>0</v>
       </c>
       <c r="U72" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A72), 1)), $C72=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V72" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A72), 1)), $C72=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C73" s="0" t="n">
         <v>1</v>
@@ -6507,16 +6726,19 @@
         <v>0</v>
       </c>
       <c r="U73" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A73), 1)), $C73=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V73" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A73), 1)), $C73=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C74" s="0" t="n">
         <v>1</v>
@@ -6587,16 +6809,19 @@
         <v>0</v>
       </c>
       <c r="U74" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A74), 1)), $C74=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V74" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A74), 1)), $C74=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>1</v>
@@ -6667,16 +6892,19 @@
         <v>0</v>
       </c>
       <c r="U75" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A75), 1)), $C75=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V75" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A75), 1)), $C75=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C76" s="0" t="n">
         <v>1</v>
@@ -6747,16 +6975,19 @@
         <v>0</v>
       </c>
       <c r="U76" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A76), 1)), $C76=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V76" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A76), 1)), $C76=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C77" s="0" t="n">
         <v>1</v>
@@ -6827,16 +7058,19 @@
         <v>0</v>
       </c>
       <c r="U77" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A77), 1)), $C77=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V77" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A77), 1)), $C77=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C78" s="0" t="n">
         <v>1</v>
@@ -6907,16 +7141,19 @@
         <v>0</v>
       </c>
       <c r="U78" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A78), 1)), $C78=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V78" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A78), 1)), $C78=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C79" s="0" t="n">
         <v>1</v>
@@ -6987,16 +7224,19 @@
         <v>0</v>
       </c>
       <c r="U79" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A79), 1)), $C79=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V79" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A79), 1)), $C79=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C80" s="0" t="n">
         <v>1</v>
@@ -7067,16 +7307,19 @@
         <v>0</v>
       </c>
       <c r="U80" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A80), 1)), $C80=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V80" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A80), 1)), $C80=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C81" s="0" t="n">
         <v>1</v>
@@ -7147,16 +7390,19 @@
         <v>0</v>
       </c>
       <c r="U81" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A81), 1)), $C81=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V81" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A81), 1)), $C81=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C82" s="0" t="n">
         <v>1</v>
@@ -7227,16 +7473,19 @@
         <v>0</v>
       </c>
       <c r="U82" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A82), 1)), $C82=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V82" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A82), 1)), $C82=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C83" s="0" t="n">
         <v>1</v>
@@ -7307,16 +7556,19 @@
         <v>0</v>
       </c>
       <c r="U83" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A83), 1)), $C83=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V83" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A83), 1)), $C83=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B84" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="B84" s="0" t="s">
-        <v>109</v>
       </c>
       <c r="C84" s="0" t="n">
         <v>1</v>
@@ -7387,16 +7639,19 @@
         <v>0</v>
       </c>
       <c r="U84" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A84), 1)), $C84=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V84" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A84), 1)), $C84=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C85" s="0" t="n">
         <v>1</v>
@@ -7467,16 +7722,19 @@
         <v>0</v>
       </c>
       <c r="U85" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A85), 1)), $C85=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V85" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A85), 1)), $C85=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C86" s="0" t="n">
         <v>1</v>
@@ -7547,16 +7805,19 @@
         <v>0</v>
       </c>
       <c r="U86" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A86), 1)), $C86=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V86" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A86), 1)), $C86=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C87" s="0" t="n">
         <v>1</v>
@@ -7627,16 +7888,19 @@
         <v>0</v>
       </c>
       <c r="U87" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A87), 1)), $C87=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V87" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A87), 1)), $C87=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C88" s="0" t="n">
         <v>1</v>
@@ -7707,16 +7971,19 @@
         <v>0</v>
       </c>
       <c r="U88" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A88), 1)), $C88=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V88" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A88), 1)), $C88=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C89" s="0" t="n">
         <v>1</v>
@@ -7787,16 +8054,19 @@
         <v>0</v>
       </c>
       <c r="U89" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A89), 1)), $C89=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V89" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A89), 1)), $C89=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>1</v>
@@ -7867,16 +8137,19 @@
         <v>0</v>
       </c>
       <c r="U90" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A90), 1)), $C90=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V90" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A90), 1)), $C90=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C91" s="0" t="n">
         <v>1</v>
@@ -7947,16 +8220,19 @@
         <v>0</v>
       </c>
       <c r="U91" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A91), 1)), $C91=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V91" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A91), 1)), $C91=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C92" s="0" t="n">
         <v>1</v>
@@ -8027,16 +8303,19 @@
         <v>0</v>
       </c>
       <c r="U92" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A92), 1)), $C92=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V92" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A92), 1)), $C92=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C93" s="0" t="n">
         <v>1</v>
@@ -8107,16 +8386,19 @@
         <v>0</v>
       </c>
       <c r="U93" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A93), 1)), $C93=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V93" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A93), 1)), $C93=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C94" s="0" t="n">
         <v>1</v>
@@ -8187,16 +8469,19 @@
         <v>0</v>
       </c>
       <c r="U94" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A94), 1)), $C94=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V94" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A94), 1)), $C94=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C95" s="0" t="n">
         <v>1</v>
@@ -8267,16 +8552,19 @@
         <v>0</v>
       </c>
       <c r="U95" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A95), 1)), $C95=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V95" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A95), 1)), $C95=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C96" s="0" t="n">
         <v>1</v>
@@ -8347,16 +8635,19 @@
         <v>0</v>
       </c>
       <c r="U96" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A96), 1)), $C96=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V96" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A96), 1)), $C96=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C97" s="0" t="n">
         <v>1</v>
@@ -8427,13 +8718,16 @@
         <v>0</v>
       </c>
       <c r="U97" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A97), 1)), $C97=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V97" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A97), 1)), $C97=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>13</v>
@@ -8507,16 +8801,19 @@
         <v>0</v>
       </c>
       <c r="U98" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A98), 1)), $C98=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V98" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A98), 1)), $C98=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C99" s="0" t="n">
         <v>1</v>
@@ -8587,13 +8884,16 @@
         <v>0</v>
       </c>
       <c r="U99" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A99), 1)), $C99=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V99" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A99), 1)), $C99=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>13</v>
@@ -8667,16 +8967,19 @@
         <v>0</v>
       </c>
       <c r="U100" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A100), 1)), $C100=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V100" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A100), 1)), $C100=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C101" s="0" t="n">
         <v>1</v>
@@ -8747,16 +9050,19 @@
         <v>0</v>
       </c>
       <c r="U101" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A101), 1)), $C101=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V101" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A101), 1)), $C101=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C102" s="0" t="n">
         <v>1</v>
@@ -8827,16 +9133,19 @@
         <v>0</v>
       </c>
       <c r="U102" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A102), 1)), $C102=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V102" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A102), 1)), $C102=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C103" s="0" t="n">
         <v>1</v>
@@ -8907,16 +9216,19 @@
         <v>0</v>
       </c>
       <c r="U103" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A103), 1)), $C103=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V103" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A103), 1)), $C103=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C104" s="0" t="n">
         <v>1</v>
@@ -8987,16 +9299,19 @@
         <v>0</v>
       </c>
       <c r="U104" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A104), 1)), $C104=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V104" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A104), 1)), $C104=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C105" s="5" t="n">
         <v>1</v>
@@ -9067,16 +9382,19 @@
         <v>0</v>
       </c>
       <c r="U105" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A105), 1)), $C105=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V105" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A105), 1)), $C105=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C106" s="0" t="n">
         <v>1</v>
@@ -9147,16 +9465,19 @@
         <v>0</v>
       </c>
       <c r="U106" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A106), 1)), $C106=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V106" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A106), 1)), $C106=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C107" s="0" t="n">
         <v>1</v>
@@ -9227,16 +9548,19 @@
         <v>0</v>
       </c>
       <c r="U107" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A107), 1)), $C107=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V107" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A107), 1)), $C107=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C108" s="0" t="n">
         <v>1</v>
@@ -9307,16 +9631,19 @@
         <v>0</v>
       </c>
       <c r="U108" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A108), 1)), $C108=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V108" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A108), 1)), $C108=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C109" s="0" t="n">
         <v>1</v>
@@ -9387,16 +9714,19 @@
         <v>0</v>
       </c>
       <c r="U109" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A109), 1)), $C109=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V109" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A109), 1)), $C109=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C110" s="0" t="n">
         <v>1</v>
@@ -9467,16 +9797,19 @@
         <v>0</v>
       </c>
       <c r="U110" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A110), 1)), $C110=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V110" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A110), 1)), $C110=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C111" s="0" t="n">
         <v>1</v>
@@ -9547,16 +9880,19 @@
         <v>0</v>
       </c>
       <c r="U111" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A111), 1)), $C111=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V111" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A111), 1)), $C111=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C112" s="0" t="n">
         <v>1</v>
@@ -9627,16 +9963,19 @@
         <v>0</v>
       </c>
       <c r="U112" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A112), 1)), $C112=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V112" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A112), 1)), $C112=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C113" s="0" t="n">
         <v>1</v>
@@ -9707,16 +10046,19 @@
         <v>0</v>
       </c>
       <c r="U113" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A113), 1)), $C113=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V113" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A113), 1)), $C113=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C114" s="4" t="n">
         <v>0</v>
@@ -9787,19 +10129,22 @@
         <v>0</v>
       </c>
       <c r="U114" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A114), 1)), $C114=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V114" s="4" t="s">
-        <v>76</v>
+        <v>0</v>
+      </c>
+      <c r="V114" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A114), 1)), $C114=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W114" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C115" s="4" t="n">
         <v>0</v>
@@ -9870,16 +10215,19 @@
         <v>0</v>
       </c>
       <c r="U115" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A115), 1)), $C115=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V115" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A115), 1)), $C115=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C116" s="4" t="n">
         <v>0</v>
@@ -9950,16 +10298,19 @@
         <v>0</v>
       </c>
       <c r="U116" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A116), 1)), $C116=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V116" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A116), 1)), $C116=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C117" s="4" t="n">
         <v>0</v>
@@ -10030,16 +10381,19 @@
         <v>0</v>
       </c>
       <c r="U117" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A117), 1)), $C117=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V117" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A117), 1)), $C117=1), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C118" s="4" t="n">
         <v>0</v>
@@ -10110,19 +10464,22 @@
         <v>0</v>
       </c>
       <c r="U118" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A118), 1)), $C118=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V118" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V118" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A118), 1)), $C118=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W118" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C119" s="4" t="n">
         <v>0</v>
@@ -10193,19 +10550,22 @@
         <v>0</v>
       </c>
       <c r="U119" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A119), 1)), $C119=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V119" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V119" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A119), 1)), $C119=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W119" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C120" s="4" t="n">
         <v>0</v>
@@ -10276,19 +10636,22 @@
         <v>0</v>
       </c>
       <c r="U120" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A120), 1)), $C120=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V120" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V120" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A120), 1)), $C120=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W120" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C121" s="4" t="n">
         <v>0</v>
@@ -10359,19 +10722,22 @@
         <v>0</v>
       </c>
       <c r="U121" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A121), 1)), $C121=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V121" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V121" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A121), 1)), $C121=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W121" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C122" s="4" t="n">
         <v>0</v>
@@ -10442,19 +10808,22 @@
         <v>0</v>
       </c>
       <c r="U122" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A122), 1)), $C122=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V122" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V122" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A122), 1)), $C122=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W122" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C123" s="4" t="n">
         <v>0</v>
@@ -10525,19 +10894,22 @@
         <v>0</v>
       </c>
       <c r="U123" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A123), 1)), $C123=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V123" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V123" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A123), 1)), $C123=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W123" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C124" s="4" t="n">
         <v>0</v>
@@ -10608,19 +10980,22 @@
         <v>0</v>
       </c>
       <c r="U124" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A124), 1)), $C124=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V124" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V124" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A124), 1)), $C124=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W124" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C125" s="4" t="n">
         <v>0</v>
@@ -10691,19 +11066,22 @@
         <v>0</v>
       </c>
       <c r="U125" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A125), 1)), $C125=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V125" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V125" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A125), 1)), $C125=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W125" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C126" s="4" t="n">
         <v>0</v>
@@ -10774,19 +11152,22 @@
         <v>0</v>
       </c>
       <c r="U126" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A126), 1)), $C126=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V126" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V126" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A126), 1)), $C126=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W126" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C127" s="4" t="n">
         <v>0</v>
@@ -10857,19 +11238,22 @@
         <v>0</v>
       </c>
       <c r="U127" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A127), 1)), $C127=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V127" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V127" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A127), 1)), $C127=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W127" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C128" s="4" t="n">
         <v>0</v>
@@ -10940,19 +11324,22 @@
         <v>0</v>
       </c>
       <c r="U128" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A128), 1)), $C128=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V128" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V128" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A128), 1)), $C128=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W128" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C129" s="4" t="n">
         <v>0</v>
@@ -11023,19 +11410,22 @@
         <v>0</v>
       </c>
       <c r="U129" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A129), 1)), $C129=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V129" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V129" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A129), 1)), $C129=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W129" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C130" s="4" t="n">
         <v>0</v>
@@ -11106,19 +11496,22 @@
         <v>0</v>
       </c>
       <c r="U130" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A130), 1)), $C130=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V130" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V130" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A130), 1)), $C130=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W130" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C131" s="4" t="n">
         <v>0</v>
@@ -11189,19 +11582,22 @@
         <v>0</v>
       </c>
       <c r="U131" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A131), 1)), $C131=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V131" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V131" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A131), 1)), $C131=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W131" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C132" s="4" t="n">
         <v>0</v>
@@ -11272,19 +11668,22 @@
         <v>0</v>
       </c>
       <c r="U132" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A132), 1)), $C132=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V132" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V132" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A132), 1)), $C132=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W132" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C133" s="4" t="n">
         <v>0</v>
@@ -11355,19 +11754,22 @@
         <v>0</v>
       </c>
       <c r="U133" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A133), 1)), $C133=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V133" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V133" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A133), 1)), $C133=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W133" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C134" s="4" t="n">
         <v>0</v>
@@ -11438,19 +11840,22 @@
         <v>0</v>
       </c>
       <c r="U134" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A134), 1)), $C134=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V134" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V134" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A134), 1)), $C134=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W134" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C135" s="4" t="n">
         <v>0</v>
@@ -11521,19 +11926,22 @@
         <v>0</v>
       </c>
       <c r="U135" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A135), 1)), $C135=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V135" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V135" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A135), 1)), $C135=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W135" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C136" s="4" t="n">
         <v>0</v>
@@ -11604,19 +12012,22 @@
         <v>0</v>
       </c>
       <c r="U136" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A136), 1)), $C136=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V136" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V136" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A136), 1)), $C136=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W136" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C137" s="4" t="n">
         <v>0</v>
@@ -11687,19 +12098,22 @@
         <v>0</v>
       </c>
       <c r="U137" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A137), 1)), $C137=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V137" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="V137" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A137), 1)), $C137=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W137" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C138" s="4" t="n">
         <v>0</v>
@@ -11770,19 +12184,22 @@
         <v>0</v>
       </c>
       <c r="U138" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A138), 1)), $C138=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V138" s="4" t="s">
-        <v>166</v>
+        <v>0</v>
+      </c>
+      <c r="V138" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A138), 1)), $C138=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W138" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C139" s="4" t="n">
         <v>0</v>
@@ -11853,19 +12270,22 @@
         <v>0</v>
       </c>
       <c r="U139" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A139), 1)), $C139=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V139" s="4" t="s">
-        <v>166</v>
+        <v>0</v>
+      </c>
+      <c r="V139" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A139), 1)), $C139=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W139" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C140" s="4" t="n">
         <v>0</v>
@@ -11936,19 +12356,22 @@
         <v>0</v>
       </c>
       <c r="U140" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A140), 1)), $C140=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V140" s="4" t="s">
-        <v>166</v>
+        <v>0</v>
+      </c>
+      <c r="V140" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A140), 1)), $C140=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W140" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C141" s="4" t="n">
         <v>0</v>
@@ -12019,19 +12442,22 @@
         <v>0</v>
       </c>
       <c r="U141" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A141), 1)), $C141=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V141" s="4" t="s">
-        <v>166</v>
+        <v>0</v>
+      </c>
+      <c r="V141" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A141), 1)), $C141=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W141" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C142" s="4" t="n">
         <v>0</v>
@@ -12102,19 +12528,22 @@
         <v>0</v>
       </c>
       <c r="U142" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A142), 1)), $C142=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V142" s="4" t="s">
-        <v>166</v>
+        <v>0</v>
+      </c>
+      <c r="V142" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A142), 1)), $C142=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W142" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C143" s="4" t="n">
         <v>0</v>
@@ -12185,19 +12614,22 @@
         <v>0</v>
       </c>
       <c r="U143" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A143), 1)), $C143=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V143" s="4" t="s">
-        <v>166</v>
+        <v>0</v>
+      </c>
+      <c r="V143" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A143), 1)), $C143=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W143" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C144" s="4" t="n">
         <v>0</v>
@@ -12268,19 +12700,22 @@
         <v>0</v>
       </c>
       <c r="U144" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A144), 1)), $C144=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V144" s="4" t="s">
-        <v>166</v>
+        <v>0</v>
+      </c>
+      <c r="V144" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A144), 1)), $C144=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W144" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C145" s="4" t="n">
         <v>0</v>
@@ -12351,19 +12786,22 @@
         <v>0</v>
       </c>
       <c r="U145" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A145), 1)), $C145=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V145" s="4" t="s">
-        <v>166</v>
+        <v>0</v>
+      </c>
+      <c r="V145" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A145), 1)), $C145=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W145" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C146" s="4" t="n">
         <v>0</v>
@@ -12434,19 +12872,22 @@
         <v>0</v>
       </c>
       <c r="U146" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A146), 1)), $C146=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V146" s="4" t="s">
-        <v>166</v>
+        <v>0</v>
+      </c>
+      <c r="V146" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A146), 1)), $C146=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W146" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C147" s="4" t="n">
         <v>0</v>
@@ -12517,19 +12958,22 @@
         <v>0</v>
       </c>
       <c r="U147" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A147), 1)), $C147=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V147" s="4" t="s">
-        <v>166</v>
+        <v>0</v>
+      </c>
+      <c r="V147" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A147), 1)), $C147=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W147" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C148" s="4" t="n">
         <v>0</v>
@@ -12600,11 +13044,14 @@
         <v>0</v>
       </c>
       <c r="U148" s="2" t="n">
-        <f aca="false">IF(AND(ISNUMBER(FIND(T(U$1), T($A148), 1)), $C148=1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V148" s="4" t="s">
-        <v>76</v>
+        <v>0</v>
+      </c>
+      <c r="V148" s="2" t="n">
+        <f aca="false">IF(AND(ISNUMBER(FIND(T(V$1), T($A148), 1)), $C148=1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W148" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -17613,7 +18060,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:U148 H2:S148 T2:U2">
+  <conditionalFormatting sqref="H3:V148 H2:S148 T2:V2">
     <cfRule type="colorScale" priority="772">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>